<commit_message>
Ajustando as distâncias para representar as direções
As direções são representadas do seguinte modo:
- 1 : Frente;
- 2 : Direita;
- 3 : Esquerda.
</commit_message>
<xml_diff>
--- a/MapeamentoIFSC/src/main/resources/Planilha_Locais.xlsx
+++ b/MapeamentoIFSC/src/main/resources/Planilha_Locais.xlsx
@@ -307,8 +307,8 @@
   </sheetPr>
   <dimension ref="A2:AX50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AX51" activeCellId="0" sqref="AX51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -534,7 +534,7 @@
         <v>1</v>
       </c>
       <c r="AF6" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,10 +568,10 @@
         <v>9</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AT12" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -579,13 +579,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AS13" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,22 +593,22 @@
         <v>11</v>
       </c>
       <c r="AN14" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AO14" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AP14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AQ14" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AU14" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AV14" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -616,13 +616,13 @@
         <v>12</v>
       </c>
       <c r="I15" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M15" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y15" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -743,7 +743,7 @@
         <v>1</v>
       </c>
       <c r="P35" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -751,7 +751,7 @@
         <v>33</v>
       </c>
       <c r="E36" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R36" s="0" t="n">
         <v>1</v>
@@ -778,70 +778,70 @@
         <v>37</v>
       </c>
       <c r="G40" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H40" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="N40" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S40" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T40" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U40" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V40" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W40" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X40" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z40" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA40" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB40" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC40" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD40" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE40" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG40" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH40" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AI40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="AL40" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AR40" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AW40" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>